<commit_message>
The process is now complete. The login feature was added in case the user was logged out in the previous session. Error handling was added. The process now reads through all tabs to check all rows of items in the excel file.
</commit_message>
<xml_diff>
--- a/Humane Society Supply List.xlsx
+++ b/Humane Society Supply List.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bioni\Documents\UiPath\NPOProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bioni\Development\NPOProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9EABA0C-0694-4CB2-A024-59E22FC04401}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A73FD96-5C60-4E01-8053-1111BBAF3374}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13224" windowHeight="5640" xr2:uid="{D50DBB5C-06FE-47F5-85D1-E1104E8C8C5C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D50DBB5C-06FE-47F5-85D1-E1104E8C8C5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Dog Food" sheetId="1" r:id="rId1"/>
     <sheet name="Dog Other" sheetId="2" r:id="rId2"/>
     <sheet name="Cat Food" sheetId="3" r:id="rId3"/>
-    <sheet name="Cat Litter" sheetId="4" r:id="rId4"/>
-    <sheet name="Cat Other" sheetId="5" r:id="rId5"/>
-    <sheet name="Misc." sheetId="6" r:id="rId6"/>
+    <sheet name="Cat Other" sheetId="5" r:id="rId4"/>
+    <sheet name="Misc." sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Cat Food'!$1:$1</definedName>
@@ -40,13 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
-  <si>
-    <t>https://www.amazon.com/Purina-Pro-Plan-Shredded-Formula/dp/B001VIYBBE/ref=sr_1_1_sspa?keywords=purina&amp;qid=1560727434&amp;s=gateway&amp;sr=8-1-spons&amp;psc=1</t>
-  </si>
-  <si>
-    <t>Qty Needed</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
   <si>
     <t>Item</t>
   </si>
@@ -55,15 +48,6 @@
   </si>
   <si>
     <t>Avg. Price</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Purina-Smartblend-Natural-Chicken-Formula/dp/B008MKI7KU/ref=sr_1_3?keywords=purina&amp;qid=1560727813&amp;s=gateway&amp;sr=8-3</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Science-Diet-Sensitive-Stomach-Chicken/dp/B003MGAIDI/ref=sxin_3_osp54-50c1bd12_cov?ascsubtag=50c1bd12-702b-4200-950a-9c6d2eabb6c5&amp;creativeASIN=B003MGAIDI&amp;cv_ct_id=amzn1.osp.50c1bd12-702b-4200-950a-9c6d2eabb6c5&amp;cv_ct_pg=search&amp;cv_ct_wn=osp-search&amp;keywords=purina&amp;linkCode=oas&amp;pd_rd_i=B003MGAIDI&amp;pd_rd_r=5627b9a6-6dff-4612-8b62-7c6e760c96cf&amp;pd_rd_w=yWzoY&amp;pd_rd_wg=Bxrs2&amp;pf_rd_p=c501273b-119a-4fc9-ad78-eda5006b0be9&amp;pf_rd_r=T0MNA2S3XG1CAKWN165W&amp;qid=1560728076&amp;s=gateway&amp;tag=42987st350sr-20</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Purina-Complete-Adult-Chicken-CHICKEN/dp/B07913DNPW/ref=sr_1_9?keywords=purina&amp;qid=1560728076&amp;s=gateway&amp;sr=8-9</t>
   </si>
   <si>
     <t>https://www.amazon.com/Pedigree-Complete-Nutrition-Grilled-Vegetable/dp/B016ZPBDFE/ref=sr_1_2?keywords=pedigree&amp;qid=1560728220&amp;s=gateway&amp;sr=8-2</t>
@@ -223,6 +207,21 @@
   </si>
   <si>
     <t>In Stock</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Purina-Pro-Plan-Shredded-Formula/dp/B001VIYBBE/ref=sr_1_1_sspa?keywords=purina&amp;qid=1560727434&amp;s=gateway&amp;sr=8-1-spons&amp;psc=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Purina-Smartblend-Natural-Chicken-Formula/dp/B008MKI7KU/ref=sr_1_3?keywords=purina&amp;qid=1560727813&amp;s=gateway&amp;sr=8-3</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Science-Diet-Sensitive-Stomach-Chicken/dp/B003MGAIDI/ref=sxin_3_osp54-50c1bd12_cov?ascsubtag=50c1bd12-702b-4200-950a-9c6d2eabb6c5&amp;creativeASIN=B003MGAIDI&amp;cv_ct_id=amzn1.osp.50c1bd12-702b-4200-950a-9c6d2eabb6c5&amp;cv_ct_pg=search&amp;cv_ct_wn=osp-search&amp;keywords=purina&amp;linkCode=oas&amp;pd_rd_i=B003MGAIDI&amp;pd_rd_r=5627b9a6-6dff-4612-8b62-7c6e760c96cf&amp;pd_rd_w=yWzoY&amp;pd_rd_wg=Bxrs2&amp;pf_rd_p=c501273b-119a-4fc9-ad78-eda5006b0be9&amp;pf_rd_r=T0MNA2S3XG1CAKWN165W&amp;qid=1560728076&amp;s=gateway&amp;tag=42987st350sr-20</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Purina-Complete-Adult-Chicken-CHICKEN/dp/B07913DNPW/ref=sr_1_9?keywords=purina&amp;qid=1560728076&amp;s=gateway&amp;sr=8-9</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -565,9 +564,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -624,6 +620,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -947,176 +946,176 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="75.6640625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="9.33203125" style="1"/>
-    <col min="8" max="8" width="47.6640625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.33203125" style="1"/>
+    <col min="3" max="3" width="9.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.7109375" style="1" customWidth="1"/>
+    <col min="6" max="7" width="9.28515625" style="1"/>
+    <col min="8" max="8" width="47.7109375" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16">
         <v>3</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D2" s="19">
         <v>45.78</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="42"/>
-    </row>
-    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="41"/>
+    </row>
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <v>4</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D3" s="14">
         <v>33.49</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="144.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <v>2</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D4" s="14">
         <v>52.99</v>
       </c>
-      <c r="E4" s="23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E4" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <v>14</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D5" s="14">
         <v>26.65</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
         <v>12</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D6" s="14">
         <v>13.74</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D7" s="14">
         <v>42.26</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
         <v>23</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D8" s="14">
         <v>9.58</v>
       </c>
       <c r="E8" s="22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="23">
+        <v>22</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="26">
+        <v>7.58</v>
+      </c>
+      <c r="E9" s="27" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="24">
-        <v>22</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="27">
-        <v>7.58</v>
-      </c>
-      <c r="E9" s="28" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1143,112 +1142,131 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="38.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="38.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.6640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="38.88671875" style="6"/>
+    <col min="1" max="1" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="38.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="8" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="32">
+    </row>
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="31">
         <v>7</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="32">
+        <v>28.16</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="33">
+        <v>12</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="29">
+        <v>22.3</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="33">
+        <v>15</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="29">
+        <v>25.48</v>
+      </c>
+      <c r="E4" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="33">
-        <v>28.16</v>
-      </c>
-      <c r="D2" s="20" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="33">
+        <v>19</v>
+      </c>
+      <c r="B5" s="30" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="34">
-        <v>12</v>
-      </c>
-      <c r="B3" s="13" t="s">
+      <c r="C5" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="29">
+        <v>7.99</v>
+      </c>
+      <c r="E5" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="30">
-        <v>22.3</v>
-      </c>
-      <c r="D3" s="22" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="34">
+        <v>5</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="35">
+        <v>24.99</v>
+      </c>
+      <c r="E6" s="42" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="34">
-        <v>15</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="30">
-        <v>25.48</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34">
-        <v>19</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="30">
-        <v>7.99</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="35">
-        <v>5</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="36">
-        <v>24.99</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{E65C6212-39C4-4BAF-8DE3-7B486A2365A0}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{518C3A79-8D36-4711-B924-665CECA6CD61}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{2D5B5B16-D2D6-4B46-B456-80DBFE959B51}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{D31D5F7C-9348-4268-AE7F-72A368BE237E}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{F8B39963-310E-49D4-A2B8-C4BBA3986F4A}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{E65C6212-39C4-4BAF-8DE3-7B486A2365A0}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{518C3A79-8D36-4711-B924-665CECA6CD61}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{2D5B5B16-D2D6-4B46-B456-80DBFE959B51}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{D31D5F7C-9348-4268-AE7F-72A368BE237E}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{50A193BC-801B-4093-8E78-729758C98074}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="70" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId6"/>
@@ -1263,102 +1281,102 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="26.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.5546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="67.88671875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="26.5546875" style="6"/>
+    <col min="1" max="1" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.5703125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="67.85546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="26.5703125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="8" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="32">
+    </row>
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="31">
         <v>14</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="32">
+        <v>29.96</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="33">
+        <v>12</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="29">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="E3" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="38" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="33">
+        <v>5</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="33">
-        <v>29.96</v>
-      </c>
-      <c r="E2" s="20" t="s">
+      <c r="C4" s="28" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="34">
-        <v>12</v>
-      </c>
-      <c r="B3" s="15" t="s">
+      <c r="D4" s="29">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="E4" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="29" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="34">
+        <v>25</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="30">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="34">
-        <v>5</v>
-      </c>
-      <c r="B4" s="15" t="s">
+      <c r="D5" s="35">
+        <v>13.89</v>
+      </c>
+      <c r="E5" s="27" t="s">
         <v>46</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="30">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="35">
-        <v>25</v>
-      </c>
-      <c r="B5" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="36">
-        <v>13.89</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1374,39 +1392,79 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FF659E-1FD0-4676-84A7-359092748599}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3254964-8B62-473A-90D8-F80BA6135357}">
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="26.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="67.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3254964-8B62-473A-90D8-F80BA6135357}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687811A2-0327-4C62-A989-CE9BF74712D6}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="26.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="67.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>